<commit_message>
adding load tests and updated play book
</commit_message>
<xml_diff>
--- a/docs/HCD/USG Playbook Checklist.xlsx
+++ b/docs/HCD/USG Playbook Checklist.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhazelbaker\Documents\GitHub\18f-prototype\docs\HCD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25940" windowHeight="15920" tabRatio="500"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="175">
   <si>
     <t>Understand what people need</t>
   </si>
@@ -381,9 +376,6 @@
   </si>
   <si>
     <t>AWS</t>
-  </si>
-  <si>
-    <t>Future enhancement</t>
   </si>
   <si>
     <t xml:space="preserve">Protractor is used for E2E testing against the browser. </t>
@@ -501,9 +493,6 @@
     <t>No personal info is collected or stored.</t>
   </si>
   <si>
-    <t xml:space="preserve">Deployment scripts used in CI and were built out for production.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">This application uses the OpenFDA dataset. </t>
   </si>
   <si>
@@ -556,6 +545,18 @@
   </si>
   <si>
     <t xml:space="preserve">Usability testers were outside of the development environment, therefore, issues/bugs/enhancements were reported to the Usability test coordinator. The usability test coordinator discussed issues with Scrum Master and Product Owner. During Sprints, issues/bugs/enhancements were entered into ScrumDo and tracked by user stories. During Sprint Stabilization issues were entered into GitHub, labeled, prioritized, worked, and tracked. </t>
+  </si>
+  <si>
+    <t>SoapUI test results exist in the Sprint Stabilzation</t>
+  </si>
+  <si>
+    <t>Deployment scripts use for CI and production. Located under devops/containers</t>
+  </si>
+  <si>
+    <t>AWS CloudWatch used</t>
+  </si>
+  <si>
+    <t>exports are possoble but not needed for this effort</t>
   </si>
 </sst>
 </file>
@@ -1134,18 +1135,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="87.33203125" style="10" customWidth="1"/>
     <col min="3" max="3" width="58" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="21">
       <c r="A1" s="2" t="s">
         <v>102</v>
       </c>
@@ -1162,63 +1163,63 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="62">
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="46.5">
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31">
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="77.5">
       <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31">
       <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="46.5">
       <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21">
       <c r="A10" s="2" t="s">
         <v>103</v>
       </c>
@@ -1235,39 +1236,39 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="31">
       <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="46.5">
       <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="31">
       <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21">
       <c r="A16" s="2" t="s">
         <v>104</v>
       </c>
@@ -1284,15 +1285,15 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="31">
       <c r="B17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18" s="10" t="s">
         <v>15</v>
       </c>
@@ -1300,47 +1301,47 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="B19" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="31">
       <c r="B20" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="B22" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="B23" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="21">
       <c r="A25" s="2" t="s">
         <v>105</v>
       </c>
@@ -1357,79 +1358,79 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="31">
       <c r="B26" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="77.5">
       <c r="B27" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="62">
       <c r="B28" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="46.5">
       <c r="B29" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="31">
       <c r="B30" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="8" customFormat="1" ht="124" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="8" customFormat="1" ht="124">
       <c r="B31" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="B32" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="B33" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="B34" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="21">
       <c r="A36" s="2" t="s">
         <v>106</v>
       </c>
@@ -1446,23 +1447,23 @@
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" s="14" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" s="14" customFormat="1" ht="46.5">
       <c r="B37" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="31">
       <c r="B38" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="B39" s="11" t="s">
         <v>34</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="31">
       <c r="B40" s="11" t="s">
         <v>35</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="B41" s="11" t="s">
         <v>36</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="31">
       <c r="B42" s="11" t="s">
         <v>37</v>
       </c>
@@ -1494,7 +1495,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="31">
       <c r="B43" s="11" t="s">
         <v>38</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="31">
       <c r="B44" s="11" t="s">
         <v>39</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="B45" s="11" t="s">
         <v>40</v>
       </c>
@@ -1518,10 +1519,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="B46" s="11"/>
     </row>
-    <row r="47" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:9" ht="21">
       <c r="A47" s="2" t="s">
         <v>107</v>
       </c>
@@ -1538,47 +1539,47 @@
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="B48" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="31">
       <c r="B49" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="31">
       <c r="B50" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="8" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="8" customFormat="1" ht="62">
       <c r="B51" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="B52" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="21">
       <c r="A54" s="1" t="s">
         <v>108</v>
       </c>
@@ -1595,71 +1596,71 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9">
       <c r="B55" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="31">
       <c r="B56" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="8" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="8" customFormat="1" ht="46.5">
       <c r="B57" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="31">
       <c r="B58" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="8" customFormat="1">
       <c r="B59" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="B60" s="10" t="s">
         <v>53</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="B61" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="B62" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="21">
       <c r="A64" s="2" t="s">
         <v>109</v>
       </c>
@@ -1676,31 +1677,31 @@
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" spans="1:9" ht="248" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="248">
       <c r="B65" s="10" t="s">
         <v>57</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="31">
       <c r="B66" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="46.5">
       <c r="B67" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="B68" s="10" t="s">
         <v>60</v>
       </c>
@@ -1708,7 +1709,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" ht="18.5">
       <c r="A70" s="2" t="s">
         <v>110</v>
       </c>
@@ -1725,7 +1726,7 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9">
       <c r="B71" s="10" t="s">
         <v>62</v>
       </c>
@@ -1733,15 +1734,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9">
       <c r="B72" s="10" t="s">
         <v>63</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="B73" s="10" t="s">
         <v>64</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9">
       <c r="B74" s="10" t="s">
         <v>65</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9">
       <c r="B75" s="10" t="s">
         <v>66</v>
       </c>
@@ -1765,15 +1766,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9">
       <c r="B76" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="B77" s="10" t="s">
         <v>68</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:9" ht="21">
       <c r="A79" s="2" t="s">
         <v>111</v>
       </c>
@@ -1798,47 +1799,47 @@
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9">
       <c r="B80" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="B81" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="46.5">
       <c r="B82" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="31">
       <c r="B83" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="14" customFormat="1">
       <c r="B84" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="18.5">
       <c r="A86" s="1" t="s">
         <v>112</v>
       </c>
@@ -1849,55 +1850,55 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" ht="31">
       <c r="B87" s="10" t="s">
         <v>76</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="31">
       <c r="B88" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="46.5">
       <c r="B89" s="10" t="s">
         <v>78</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="31">
       <c r="B90" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="B91" s="10" t="s">
         <v>80</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" s="14" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="14" customFormat="1" ht="30">
       <c r="B92" s="15" t="s">
         <v>81</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" s="14" customFormat="1" ht="18.5">
       <c r="A94" s="17" t="s">
         <v>113</v>
       </c>
@@ -1908,55 +1909,69 @@
         <v>101</v>
       </c>
     </row>
-    <row r="95" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" s="14" customFormat="1">
       <c r="B95" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C95" s="15"/>
-    </row>
-    <row r="96" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C95" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" s="14" customFormat="1">
       <c r="B96" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C96" s="15"/>
-    </row>
-    <row r="97" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C96" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" s="14" customFormat="1">
       <c r="B97" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C97" s="15"/>
-    </row>
-    <row r="98" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C97" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" s="14" customFormat="1">
       <c r="B98" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C98" s="15"/>
-    </row>
-    <row r="99" spans="1:3" s="14" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="C98" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" s="14" customFormat="1" ht="30">
       <c r="B99" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C99" s="15"/>
-    </row>
-    <row r="100" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C99" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" s="14" customFormat="1">
       <c r="B100" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C100" s="15"/>
-    </row>
-    <row r="101" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C100" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" s="14" customFormat="1">
       <c r="B101" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C101" s="15"/>
-    </row>
-    <row r="102" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C101" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" s="14" customFormat="1">
       <c r="B102" s="15" t="s">
         <v>90</v>
       </c>
       <c r="C102" s="15"/>
     </row>
-    <row r="104" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:3" ht="18.5">
       <c r="A104" s="1" t="s">
         <v>114</v>
       </c>
@@ -1967,79 +1982,79 @@
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="8" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" s="8" customFormat="1" ht="108.5">
       <c r="B105" s="12" t="s">
         <v>92</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" s="8" customFormat="1" ht="31">
       <c r="B106" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="31">
       <c r="B107" s="10" t="s">
         <v>94</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="31">
       <c r="B108" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="31">
       <c r="B109" s="10" t="s">
         <v>96</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="31">
       <c r="B110" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" s="14" customFormat="1">
       <c r="B111" s="15" t="s">
         <v>98</v>
       </c>
       <c r="C111" s="15"/>
     </row>
-    <row r="112" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" ht="31">
       <c r="B112" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" ht="31">
       <c r="B113" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>